<commit_message>
11 May 2024 Selenium Data Driven
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AutomationDemoSIte.xlsx
+++ b/src/test/resources/TestData/AutomationDemoSIte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\SDETSeleniumJavaMarch2024\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\SDETSeleniumJavaMarch2024\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7130C9-4B8B-452E-BB5B-BCABBDEE510D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CEA4F-87CA-4290-8304-2D70BC40E12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -328,12 +328,16 @@
   </si>
   <si>
     <t>Geetha</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -707,20 +711,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.08984375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.81640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.6328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.6328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -783,52 +787,52 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>9876543210</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="0">
         <v>1987</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="0">
         <v>5</v>
       </c>
       <c r="Q2" s="2" t="s">
@@ -837,54 +841,57 @@
       <c r="R2" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="S2" t="s" s="0">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>9876543211</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="0">
         <v>1988</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="0">
         <v>9</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -895,52 +902,52 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>9876543212</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="0">
         <v>1989</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="0">
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
@@ -949,54 +956,57 @@
       <c r="R4" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="S4" t="s" s="0">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>9876543213</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="0">
         <v>1990</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="0">
         <v>18</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -1007,52 +1017,52 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>9876543214</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="0">
         <v>1991</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="0">
         <v>21</v>
       </c>
       <c r="Q6" s="2" t="s">
@@ -1061,54 +1071,57 @@
       <c r="R6" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="S6" t="s" s="0">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>9876543215</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="0">
         <v>1992</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="0">
         <v>27</v>
       </c>
       <c r="Q7" s="2" t="s">
@@ -1119,52 +1132,52 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>35</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>9876543216</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="0">
         <v>1993</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="0">
         <v>30</v>
       </c>
       <c r="Q8" s="2" t="s">
@@ -1172,6 +1185,9 @@
       </c>
       <c r="R8" s="2" t="s">
         <v>88</v>
+      </c>
+      <c r="S8" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>